<commit_message>
Het Testscipt is nu up to date
</commit_message>
<xml_diff>
--- a/m_TEMPLATE_TestScript.xlsx
+++ b/m_TEMPLATE_TestScript.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Repositories\Eindopdracht-Bi6a-Huberts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Step</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Geen error</t>
   </si>
   <si>
-    <t>Om eerlijk te zijn: de namen komen niet altijd overeen met de ID's.</t>
-  </si>
-  <si>
     <t>MP3-Bestand openen</t>
   </si>
   <si>
@@ -147,16 +144,13 @@
     <t>Filteren op Classificatie via filterbalk</t>
   </si>
   <si>
-    <t>Ik heb ervoor gekozen dat het niet zal lukken</t>
-  </si>
-  <si>
-    <t>In de code zelf is hierover commentaar opgenomen</t>
-  </si>
-  <si>
     <t>Sorteren op ID via sortering</t>
   </si>
   <si>
     <t>Sorteren op Aantal Hosts via sortering</t>
+  </si>
+  <si>
+    <t>Er is een rare bug waardoor eerst te klikken op sorteren op aantal hosts en dan sorteren op Classificatie de GUI blijft hangen op de sortering op aantal hosts. Dit kan verholpen worden door weer te sorteren op ID.</t>
   </si>
 </sst>
 </file>
@@ -771,21 +765,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -824,6 +803,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1172,7 +1166,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:H20"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1187,16 +1181,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49" t="s">
+      <c r="A1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="51"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -1206,11 +1200,11 @@
       <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="56"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="51"/>
       <c r="G2" s="5"/>
       <c r="H2" s="6"/>
     </row>
@@ -1219,13 +1213,13 @@
       <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="56"/>
       <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1233,11 +1227,11 @@
       <c r="B4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="61"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1245,11 +1239,11 @@
       <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="61"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="56"/>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1257,13 +1251,13 @@
       <c r="B6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59"/>
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1280,7 +1274,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="20">
-        <v>43138</v>
+        <v>43159</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -1317,10 +1311,10 @@
       <c r="F9" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="58"/>
+      <c r="H9" s="53"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="33">
@@ -1337,8 +1331,8 @@
       </c>
       <c r="E10" s="35"/>
       <c r="F10" s="35"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="53"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="48"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="33">
@@ -1381,7 +1375,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="34" t="s">
         <v>29</v>
@@ -1391,9 +1385,7 @@
       </c>
       <c r="E13" s="35"/>
       <c r="F13" s="35"/>
-      <c r="G13" s="62" t="s">
-        <v>30</v>
-      </c>
+      <c r="G13" s="62"/>
       <c r="H13" s="63"/>
     </row>
     <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1401,7 +1393,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>26</v>
@@ -1419,7 +1411,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="34" t="s">
         <v>29</v>
@@ -1432,22 +1424,24 @@
       <c r="G15" s="40"/>
       <c r="H15" s="41"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="33">
         <v>7</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="35" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
-      <c r="G16" s="40"/>
+      <c r="G16" s="40" t="s">
+        <v>38</v>
+      </c>
       <c r="H16" s="41"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1455,19 +1449,17 @@
         <v>8</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D17" s="35" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="35"/>
       <c r="F17" s="35"/>
-      <c r="G17" s="40" t="s">
-        <v>38</v>
-      </c>
+      <c r="G17" s="40"/>
       <c r="H17" s="41"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1475,10 +1467,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="35" t="s">
         <v>27</v>
@@ -1493,10 +1485,10 @@
         <v>10</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="35" t="s">
         <v>27</v>
@@ -1590,7 +1582,7 @@
       <c r="G26" s="40"/>
       <c r="H26" s="41"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33">
         <v>18</v>
       </c>
@@ -1599,8 +1591,8 @@
       <c r="D27" s="35"/>
       <c r="E27" s="35"/>
       <c r="F27" s="35"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="41"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="61"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="33">
@@ -1611,8 +1603,6 @@
       <c r="D28" s="35"/>
       <c r="E28" s="35"/>
       <c r="F28" s="35"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="41"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="33">
@@ -1623,8 +1613,6 @@
       <c r="D29" s="35"/>
       <c r="E29" s="35"/>
       <c r="F29" s="35"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="41"/>
     </row>
     <row r="30" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="36"/>
@@ -1635,16 +1623,24 @@
       <c r="D30" s="39"/>
       <c r="E30" s="39"/>
       <c r="F30" s="39"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
+  <mergeCells count="26">
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
     <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G19:H19"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="G10:H10"/>
@@ -1653,22 +1649,9 @@
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C5:G5"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>